<commit_message>
data analysis + graphs + code update
</commit_message>
<xml_diff>
--- a/Prototype testing/Nunchuck model/20210930-221200.xlsx
+++ b/Prototype testing/Nunchuck model/20210930-221200.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorn\Documents\GitHub\BUG\Prototype testing\Nunchuck model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\Documents\GitHub\BUG\Prototype testing\Nunchuck model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D33BA1A5-BCA7-443C-80B8-78C71936CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3F79A1-7961-47F8-8AF8-757718104DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20210930-221200" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,111 +646,123 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'20210930-221200'!$F$2:$F$35</c:f>
+              <c:f>'20210930-221200'!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.92523148148148149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92546296296296293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92569444444444438</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92592592592592582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92615740740740726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92638888888888871</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92662037037037015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92685185185185159</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92708333333333304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92731481481481448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92754629629629592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92777777777777737</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92800925925925881</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92824074074074026</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9284722222222217</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92870370370370314</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92893518518518459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92916666666666603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92939814814814747</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92962962962962892</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92986111111111036</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9300925925925918</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93032407407407325</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93055555555555469</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93078703703703614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93101851851851758</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93124999999999902</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93148148148148047</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93171296296296191</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93194444444444335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9321759259259248</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93240740740740624</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93263888888888768</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93287037037036913</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93310185185185057</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93333333333333202</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93356481481481346</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9337962962962949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -886,111 +909,123 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'20210930-221200'!$F$2:$F$35</c:f>
+              <c:f>'20210930-221200'!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.92523148148148149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92546296296296293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92569444444444438</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92592592592592582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92615740740740726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92638888888888871</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92662037037037015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92685185185185159</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92708333333333304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92731481481481448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92754629629629592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92777777777777737</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92800925925925881</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92824074074074026</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9284722222222217</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92870370370370314</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92893518518518459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92916666666666603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92939814814814747</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92962962962962892</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92986111111111036</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9300925925925918</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93032407407407325</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93055555555555469</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93078703703703614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93101851851851758</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93124999999999902</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93148148148148047</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93171296296296191</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93194444444444335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9321759259259248</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93240740740740624</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93263888888888768</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93287037037036913</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93310185185185057</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93333333333333202</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93356481481481346</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9337962962962949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,111 +1172,123 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'20210930-221200'!$F$2:$F$35</c:f>
+              <c:f>'20210930-221200'!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.92523148148148149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92546296296296293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92569444444444438</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92592592592592582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92615740740740726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92638888888888871</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92662037037037015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92685185185185159</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92708333333333304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92731481481481448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92754629629629592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92777777777777737</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92800925925925881</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92824074074074026</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9284722222222217</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92870370370370314</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92893518518518459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92916666666666603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92939814814814747</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92962962962962892</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92986111111111036</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9300925925925918</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93032407407407325</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93055555555555469</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93078703703703614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93101851851851758</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93124999999999902</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93148148148148047</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93171296296296191</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93194444444444335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9321759259259248</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93240740740740624</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93263888888888768</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93287037037036913</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93310185185185057</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93333333333333202</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93356481481481346</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9337962962962949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1388,111 +1435,123 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'20210930-221200'!$F$2:$F$35</c:f>
+              <c:f>'20210930-221200'!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.92523148148148149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92546296296296293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92569444444444438</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92592592592592582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92615740740740726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92638888888888871</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92662037037037015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92685185185185159</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92708333333333304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92731481481481448</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92754629629629592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92777777777777737</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92800925925925881</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92824074074074026</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9284722222222217</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92870370370370314</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92893518518518459</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92916666666666603</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92939814814814747</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92962962962962892</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.92986111111111036</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9300925925925918</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93032407407407325</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93055555555555469</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93078703703703614</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93101851851851758</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93124999999999902</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93148148148148047</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93171296296296191</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93194444444444335</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.9321759259259248</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93240740740740624</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93263888888888768</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>0.93287037037036913</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.93310185185185057</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.93333333333333202</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.93356481481481346</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9337962962962949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1666,7 +1725,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="606794079"/>
@@ -1725,7 +1784,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="606791999"/>
@@ -1767,7 +1826,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1804,7 +1863,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2380,16 +2439,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2713,11 +2772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V566"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>